<commit_message>
app ready for relase. (finally)
</commit_message>
<xml_diff>
--- a/StudentResult.xlsx
+++ b/StudentResult.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xxjos\Desktop\SelectorEstudiantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D564F791-A6AE-4DED-90D8-5D059529F779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82DDDC7-1020-453D-A3DD-73F90FB36447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Desarrollador en vivo</t>
   </si>
@@ -29,14 +29,55 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Alex Jose Rodriguez Taveras</t>
+  </si>
+  <si>
+    <t>Ashlee Ramirez Rosario</t>
+  </si>
+  <si>
+    <t>2024-07-11 20:17:06</t>
+  </si>
+  <si>
+    <t>Oscar Daniel Tuletta Mercedes</t>
+  </si>
+  <si>
+    <t>Jamil Guzman Feliz</t>
+  </si>
+  <si>
+    <t>2024-07-11 20:22:52</t>
+  </si>
+  <si>
+    <t>Rafael Antonio Urbaez Hernandez</t>
+  </si>
+  <si>
+    <t>2024-07-11 20:32:27</t>
+  </si>
+  <si>
+    <t>Cyd Marie Jorge Chapman</t>
+  </si>
+  <si>
+    <t>Edison Yadir Rossis</t>
+  </si>
+  <si>
+    <t>2024-07-11 20:33:23</t>
+  </si>
+  <si>
+    <t>Yoelmi Alexander Alcala Valdez</t>
+  </si>
+  <si>
+    <t>Yadianna Vargas Pimentel</t>
+  </si>
+  <si>
+    <t>2024-07-11 20:33:50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -398,32 +439,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
app relase, first bug fix.
</commit_message>
<xml_diff>
--- a/StudentResult.xlsx
+++ b/StudentResult.xlsx
@@ -15,12 +15,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Desarrollador en vivo</t>
   </si>
@@ -30,54 +30,13 @@
   <si>
     <t>Fecha</t>
   </si>
-  <si>
-    <t>Alex Jose Rodriguez Taveras</t>
-  </si>
-  <si>
-    <t>Ashlee Ramirez Rosario</t>
-  </si>
-  <si>
-    <t>2024-07-11 20:17:06</t>
-  </si>
-  <si>
-    <t>Oscar Daniel Tuletta Mercedes</t>
-  </si>
-  <si>
-    <t>Jamil Guzman Feliz</t>
-  </si>
-  <si>
-    <t>2024-07-11 20:22:52</t>
-  </si>
-  <si>
-    <t>Rafael Antonio Urbaez Hernandez</t>
-  </si>
-  <si>
-    <t>2024-07-11 20:32:27</t>
-  </si>
-  <si>
-    <t>Cyd Marie Jorge Chapman</t>
-  </si>
-  <si>
-    <t>Edison Yadir Rossis</t>
-  </si>
-  <si>
-    <t>2024-07-11 20:33:23</t>
-  </si>
-  <si>
-    <t>Yoelmi Alexander Alcala Valdez</t>
-  </si>
-  <si>
-    <t>Yadianna Vargas Pimentel</t>
-  </si>
-  <si>
-    <t>2024-07-11 20:33:50</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -439,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
@@ -447,78 +406,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>